<commit_message>
Revert "Worked on BOMs"
This reverts commit a2125976a54354ab525f3884e5189c7120c6e01c.
</commit_message>
<xml_diff>
--- a/Documentation/UPCB_BOM.xlsx
+++ b/Documentation/UPCB_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="4155" windowWidth="25230" windowHeight="4170"/>
+    <workbookView xWindow="-15" yWindow="6240" windowWidth="25230" windowHeight="6300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Column10</t>
   </si>
@@ -81,6 +81,9 @@
     <t>Header</t>
   </si>
   <si>
+    <t>Molex</t>
+  </si>
+  <si>
     <t>Crimp Pins</t>
   </si>
   <si>
@@ -96,6 +99,21 @@
     <t>5 pin polar</t>
   </si>
   <si>
+    <t>PRT-08098</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/8098</t>
+  </si>
+  <si>
+    <t>22-23-2051</t>
+  </si>
+  <si>
+    <t>PRT-08230</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/8230</t>
+  </si>
+  <si>
     <t>Adafruit</t>
   </si>
   <si>
@@ -109,42 +127,6 @@
   </si>
   <si>
     <t>Cape</t>
-  </si>
-  <si>
-    <t>Transistor</t>
-  </si>
-  <si>
-    <t>NPN</t>
-  </si>
-  <si>
-    <t>Fairchild Semiconductor</t>
-  </si>
-  <si>
-    <t>2N3904TFR</t>
-  </si>
-  <si>
-    <t>Digikey</t>
-  </si>
-  <si>
-    <t>2N3904D26ZCT-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/2N3904TFR/2N3904D26ZCT-ND/458921</t>
-  </si>
-  <si>
-    <t>Molex Inc</t>
-  </si>
-  <si>
-    <t>WM4203-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/0022232051/WM4203-ND/26673</t>
-  </si>
-  <si>
-    <t>WM2014-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/scripts/dksearch/dksus.dll?vendor=0&amp;keywords=22-01-2057</t>
   </si>
 </sst>
 </file>
@@ -578,7 +560,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:I5"/>
+      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +572,7 @@
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="74" customWidth="1"/>
+    <col min="8" max="8" width="82.28515625" customWidth="1"/>
     <col min="9" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
     <col min="12" max="15" width="12" hidden="1" customWidth="1"/>
@@ -652,19 +634,19 @@
         <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G2" s="4">
         <v>572</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="I2" s="5">
         <v>9.9499999999999993</v>
@@ -689,10 +671,10 @@
         <v>18</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="I3" s="5">
         <v>9.9499999999999993</v>
@@ -710,32 +692,32 @@
         <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="4">
-        <v>22232051</v>
+        <v>26</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="I4" s="5">
-        <v>0.42</v>
+        <v>0.45</v>
       </c>
       <c r="J4" s="3">
         <v>10</v>
       </c>
       <c r="K4" s="2">
         <f>Table3[[#This Row],[Price]]*Table3[[#This Row],[Quantity]]</f>
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -743,41 +725,39 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="4">
-        <v>22012057</v>
-      </c>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="I5" s="5">
-        <v>0.27</v>
+        <v>0.45</v>
       </c>
       <c r="J5" s="3">
         <v>20</v>
       </c>
       <c r="K5" s="2">
         <f>Table3[[#This Row],[Price]]*Table3[[#This Row],[Quantity]]</f>
-        <v>5.4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3">
         <v>20</v>
@@ -788,10 +768,10 @@
         <v>18</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I6" s="5">
         <v>1.95</v>
@@ -805,37 +785,19 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0.19</v>
-      </c>
-      <c r="J7" s="3">
-        <v>5</v>
-      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="3"/>
       <c r="K7" s="2">
         <f>Table3[[#This Row],[Price]]*Table3[[#This Row],[Quantity]]</f>
-        <v>0.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1035,7 +997,7 @@
       <c r="J21" s="6"/>
       <c r="K21" s="7">
         <f>SUM(Table3[Total])</f>
-        <v>40.200000000000003</v>
+        <v>43.15</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1203,24 +1165,17 @@
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="http://www.adafruit.com/products/572"/>
     <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="H6" r:id="rId3"/>
-    <hyperlink ref="G6" r:id="rId4"/>
-    <hyperlink ref="D7" r:id="rId5" display="http://digikey.com/Suppliers/us/Fairchild-Semiconductor.page?lang=en"/>
-    <hyperlink ref="E7" r:id="rId6" display="http://www.digikey.com/product-detail/en/2N3904TFR/2N3904D26ZCT-ND/458921"/>
-    <hyperlink ref="G7" r:id="rId7" display="http://www.digikey.com/product-detail/en/2N3904TFR/2N3904D26ZCT-ND/458921"/>
-    <hyperlink ref="H7" r:id="rId8"/>
-    <hyperlink ref="D4" r:id="rId9" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
-    <hyperlink ref="E4" r:id="rId10" display="http://www.digikey.com/product-detail/en/0022232051/WM4203-ND/26673"/>
-    <hyperlink ref="G4" r:id="rId11" display="http://www.digikey.com/product-detail/en/0022232051/WM4203-ND/26673"/>
-    <hyperlink ref="H4" r:id="rId12"/>
-    <hyperlink ref="D5" r:id="rId13" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
-    <hyperlink ref="G5" r:id="rId14"/>
-    <hyperlink ref="E5" r:id="rId15" display="http://www.digikey.com/scripts/dksearch/dksus.dll?vendor=0&amp;keywords=22-01-2057"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="H4" r:id="rId4"/>
+    <hyperlink ref="H5" r:id="rId5"/>
+    <hyperlink ref="G5" r:id="rId6"/>
+    <hyperlink ref="H6" r:id="rId7"/>
+    <hyperlink ref="G6" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
   <tableParts count="1">
-    <tablePart r:id="rId17"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Revert "Revert "Worked on BOMs""
This reverts commit 5e8def40d806edfa2d7bb324aa1a0e359af96b65.
</commit_message>
<xml_diff>
--- a/Documentation/UPCB_BOM.xlsx
+++ b/Documentation/UPCB_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6240" windowWidth="25230" windowHeight="6300"/>
+    <workbookView xWindow="-15" yWindow="4155" windowWidth="25230" windowHeight="4170"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>Column10</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Header</t>
   </si>
   <si>
-    <t>Molex</t>
-  </si>
-  <si>
     <t>Crimp Pins</t>
   </si>
   <si>
@@ -99,21 +96,6 @@
     <t>5 pin polar</t>
   </si>
   <si>
-    <t>PRT-08098</t>
-  </si>
-  <si>
-    <t>https://www.sparkfun.com/products/8098</t>
-  </si>
-  <si>
-    <t>22-23-2051</t>
-  </si>
-  <si>
-    <t>PRT-08230</t>
-  </si>
-  <si>
-    <t>https://www.sparkfun.com/products/8230</t>
-  </si>
-  <si>
     <t>Adafruit</t>
   </si>
   <si>
@@ -127,6 +109,42 @@
   </si>
   <si>
     <t>Cape</t>
+  </si>
+  <si>
+    <t>Transistor</t>
+  </si>
+  <si>
+    <t>NPN</t>
+  </si>
+  <si>
+    <t>Fairchild Semiconductor</t>
+  </si>
+  <si>
+    <t>2N3904TFR</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>2N3904D26ZCT-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/2N3904TFR/2N3904D26ZCT-ND/458921</t>
+  </si>
+  <si>
+    <t>Molex Inc</t>
+  </si>
+  <si>
+    <t>WM4203-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/0022232051/WM4203-ND/26673</t>
+  </si>
+  <si>
+    <t>WM2014-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/scripts/dksearch/dksus.dll?vendor=0&amp;keywords=22-01-2057</t>
   </si>
 </sst>
 </file>
@@ -560,7 +578,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +590,7 @@
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="82.28515625" customWidth="1"/>
+    <col min="8" max="8" width="74" customWidth="1"/>
     <col min="9" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
     <col min="12" max="15" width="12" hidden="1" customWidth="1"/>
@@ -634,19 +652,19 @@
         <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G2" s="4">
         <v>572</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I2" s="5">
         <v>9.9499999999999993</v>
@@ -671,10 +689,10 @@
         <v>18</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I3" s="5">
         <v>9.9499999999999993</v>
@@ -692,32 +710,32 @@
         <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="4">
+        <v>22232051</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I4" s="5">
-        <v>0.45</v>
+        <v>0.42</v>
       </c>
       <c r="J4" s="3">
         <v>10</v>
       </c>
       <c r="K4" s="2">
         <f>Table3[[#This Row],[Price]]*Table3[[#This Row],[Quantity]]</f>
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -725,39 +743,41 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="3"/>
+      <c r="D5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="4">
+        <v>22012057</v>
+      </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="I5" s="5">
-        <v>0.45</v>
+        <v>0.27</v>
       </c>
       <c r="J5" s="3">
         <v>20</v>
       </c>
       <c r="K5" s="2">
         <f>Table3[[#This Row],[Price]]*Table3[[#This Row],[Quantity]]</f>
-        <v>9</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="C6" s="3">
         <v>20</v>
@@ -768,10 +788,10 @@
         <v>18</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="I6" s="5">
         <v>1.95</v>
@@ -785,19 +805,37 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="3"/>
+      <c r="D7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="J7" s="3">
+        <v>5</v>
+      </c>
       <c r="K7" s="2">
         <f>Table3[[#This Row],[Price]]*Table3[[#This Row],[Quantity]]</f>
-        <v>0</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -997,7 +1035,7 @@
       <c r="J21" s="6"/>
       <c r="K21" s="7">
         <f>SUM(Table3[Total])</f>
-        <v>43.15</v>
+        <v>40.200000000000003</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1165,17 +1203,24 @@
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="http://www.adafruit.com/products/572"/>
     <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="H4" r:id="rId4"/>
-    <hyperlink ref="H5" r:id="rId5"/>
-    <hyperlink ref="G5" r:id="rId6"/>
-    <hyperlink ref="H6" r:id="rId7"/>
-    <hyperlink ref="G6" r:id="rId8"/>
+    <hyperlink ref="H6" r:id="rId3"/>
+    <hyperlink ref="G6" r:id="rId4"/>
+    <hyperlink ref="D7" r:id="rId5" display="http://digikey.com/Suppliers/us/Fairchild-Semiconductor.page?lang=en"/>
+    <hyperlink ref="E7" r:id="rId6" display="http://www.digikey.com/product-detail/en/2N3904TFR/2N3904D26ZCT-ND/458921"/>
+    <hyperlink ref="G7" r:id="rId7" display="http://www.digikey.com/product-detail/en/2N3904TFR/2N3904D26ZCT-ND/458921"/>
+    <hyperlink ref="H7" r:id="rId8"/>
+    <hyperlink ref="D4" r:id="rId9" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
+    <hyperlink ref="E4" r:id="rId10" display="http://www.digikey.com/product-detail/en/0022232051/WM4203-ND/26673"/>
+    <hyperlink ref="G4" r:id="rId11" display="http://www.digikey.com/product-detail/en/0022232051/WM4203-ND/26673"/>
+    <hyperlink ref="H4" r:id="rId12"/>
+    <hyperlink ref="D5" r:id="rId13" display="http://digikey.com/Suppliers/us/Molex.page?lang=en"/>
+    <hyperlink ref="G5" r:id="rId14"/>
+    <hyperlink ref="E5" r:id="rId15" display="http://www.digikey.com/scripts/dksearch/dksus.dll?vendor=0&amp;keywords=22-01-2057"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>